<commit_message>
progetto linguaggi parte B, finita tabella slr
</commit_message>
<xml_diff>
--- a/Bruniera/linguaggi e compilatori/progetto/parteB/slr.xlsx
+++ b/Bruniera/linguaggi e compilatori/progetto/parteB/slr.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>ACTION</t>
   </si>
@@ -120,6 +120,9 @@
     <t>e8</t>
   </si>
   <si>
+    <t>e15</t>
+  </si>
+  <si>
     <t>I4</t>
   </si>
   <si>
@@ -144,6 +147,9 @@
     <t>I6</t>
   </si>
   <si>
+    <t>e12</t>
+  </si>
+  <si>
     <t>I7</t>
   </si>
   <si>
@@ -159,9 +165,15 @@
     <t>s13</t>
   </si>
   <si>
+    <t>e14</t>
+  </si>
+  <si>
     <t>I9</t>
   </si>
   <si>
+    <t>e13</t>
+  </si>
+  <si>
     <t>I10</t>
   </si>
   <si>
@@ -216,9 +228,15 @@
     <t>r3</t>
   </si>
   <si>
+    <t>e16</t>
+  </si>
+  <si>
     <t>I19</t>
   </si>
   <si>
+    <t>r4</t>
+  </si>
+  <si>
     <t xml:space="preserve">print "internal error"; panic</t>
   </si>
   <si>
@@ -237,7 +255,7 @@
     <t xml:space="preserve">print "unexpected {lookahead}"; skip</t>
   </si>
   <si>
-    <t xml:space="preserve">print "missing expression"; goto I4</t>
+    <t xml:space="preserve">print "missing expression"; push E; goto I4</t>
   </si>
   <si>
     <t xml:space="preserve">print "incomplete program"; panic</t>
@@ -252,16 +270,19 @@
     <t xml:space="preserve">print "missing }"; add }</t>
   </si>
   <si>
-    <t>e12</t>
-  </si>
-  <si>
-    <t>e13</t>
-  </si>
-  <si>
-    <t>e14</t>
-  </si>
-  <si>
-    <t>e15</t>
+    <t xml:space="preserve">print "missing expression"; push E; goto I10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print "missing expression"; push E; goto I14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print "unexpected {TOS}"; drop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print "double statement"; drop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">print "missing id"; pop X; push id; push I13; push X: goto I18</t>
   </si>
 </sst>
 </file>
@@ -365,10 +386,10 @@
     </xf>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="3" fillId="4" borderId="1" numFmtId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,13 +992,13 @@
       <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="4" t="s">
@@ -986,13 +1007,13 @@
       <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="6">
         <v>1</v>
       </c>
       <c r="M4" s="4" t="s">
@@ -1033,16 +1054,24 @@
       <c r="I5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="L5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="3" t="s">
@@ -1060,7 +1089,7 @@
       <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1069,25 +1098,33 @@
       <c r="H6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="L6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1099,7 +1136,7 @@
       <c r="E7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -1117,39 +1154,43 @@
       <c r="K7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="5">
+      <c r="L7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="6">
         <v>4</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="G8" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="5" t="s">
         <v>39</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>17</v>
@@ -1160,35 +1201,43 @@
       <c r="K8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="L8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>41</v>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>41</v>
+      <c r="H9" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>17</v>
@@ -1199,198 +1248,328 @@
       <c r="K9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="L9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="G10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="J10" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="5">
+      <c r="L10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="6">
         <v>10</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="6">
         <v>11</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="J11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+      <c r="L11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
       <c r="A12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="J12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="5">
+      <c r="L12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="6">
         <v>12</v>
       </c>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
+      <c r="N12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" ht="14.25">
       <c r="A13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="5" t="s">
+      <c r="C13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="J13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="5">
+      <c r="L13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N13" s="6">
         <v>14</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+        <v>53</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="J14" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+      <c r="L14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" ht="14.25">
       <c r="A15" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="J15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="L15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>34</v>
@@ -1398,167 +1577,281 @@
       <c r="K16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="L16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
+      <c r="H17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="J17" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="5">
+      <c r="L17" s="6">
         <v>18</v>
       </c>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="M17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="J18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="L18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="J19" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="L19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="J20" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="L20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="L21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>34</v>
@@ -1566,157 +1859,200 @@
       <c r="K22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="1"/>
-      <c r="M22" s="5">
+      <c r="L22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M22" s="6">
         <v>19</v>
       </c>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="N22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="J23" s="4" t="s">
         <v>34</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
+      <c r="L23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="24" ht="14.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="8"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="8"/>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>69</v>
+      <c r="B27" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>70</v>
+      <c r="B28" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>71</v>
+      <c r="B29" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>72</v>
+      <c r="B30" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>73</v>
+      <c r="B31" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>74</v>
+      <c r="B32" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>75</v>
+      <c r="B33" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>76</v>
+        <v>48</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35" ht="14.25">
       <c r="A35" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>77</v>
+        <v>37</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>78</v>
+        <v>39</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="37" ht="14.25">
       <c r="A37" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B37" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="38" ht="14.25">
       <c r="A38" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="40" ht="14.25">
       <c r="A40" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" ht="14.25"/>
+        <v>35</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="A41" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:J2"/>

</xml_diff>